<commit_message>
added bio to script
</commit_message>
<xml_diff>
--- a/diet_groups_male.xlsx
+++ b/diet_groups_male.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,175 +498,150 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CH4</t>
+          <t>Bio</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8711031476445004</v>
+        <v>262.1093884855168</v>
       </c>
       <c r="C3" t="n">
-        <v>1.11307376761667</v>
+        <v>279.1467580569499</v>
       </c>
       <c r="D3" t="n">
-        <v>2.500159873131</v>
+        <v>431.1378158502502</v>
       </c>
       <c r="E3" t="n">
-        <v>1.536385408702169</v>
+        <v>325.0836925024324</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1451056996828334</v>
+        <v>123.783734336585</v>
       </c>
       <c r="G3" t="n">
-        <v>0.7825921710713336</v>
+        <v>256.3340692038661</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>N2O</t>
+          <t>LandUsed</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.3459226631293337</v>
+        <v>7.064051100569848</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4047201963606667</v>
+        <v>8.89832531005036</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8608601118685016</v>
+        <v>24.48120934962563</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5480558191668324</v>
+        <v>13.41315505483782</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2191429246239998</v>
+        <v>4.560443602925329</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3113943101230001</v>
+        <v>6.715724361482192</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>LandUsed</t>
+          <t>WaterScarcity</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7.064051100569848</v>
+        <v>18989.04397999006</v>
       </c>
       <c r="C5" t="n">
-        <v>8.89832531005036</v>
+        <v>17987.99032789875</v>
       </c>
       <c r="D5" t="n">
-        <v>24.48120934962563</v>
+        <v>22863.18271384005</v>
       </c>
       <c r="E5" t="n">
-        <v>13.41315505483782</v>
+        <v>19461.57485078338</v>
       </c>
       <c r="F5" t="n">
-        <v>4.560443602925329</v>
+        <v>15593.92534567281</v>
       </c>
       <c r="G5" t="n">
-        <v>6.715724361482192</v>
+        <v>16813.84903151101</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>WaterScarcity</t>
+          <t>Eutrophication</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>18989.04397999006</v>
+        <v>22.42153102407176</v>
       </c>
       <c r="C6" t="n">
-        <v>17987.99032789875</v>
+        <v>24.64301369893336</v>
       </c>
       <c r="D6" t="n">
-        <v>22863.18271384005</v>
+        <v>44.01964698086995</v>
       </c>
       <c r="E6" t="n">
-        <v>19461.57485078338</v>
+        <v>31.12128529111659</v>
       </c>
       <c r="F6" t="n">
-        <v>15593.92534567281</v>
+        <v>11.58014932273346</v>
       </c>
       <c r="G6" t="n">
-        <v>16813.84903151101</v>
+        <v>18.36717080568337</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Eutrophication</t>
+          <t>WaterUse</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>22.42153102407176</v>
+        <v>817.9715822192637</v>
       </c>
       <c r="C7" t="n">
-        <v>24.64301369893336</v>
+        <v>787.2341085736156</v>
       </c>
       <c r="D7" t="n">
-        <v>44.01964698086995</v>
+        <v>984.7551522402184</v>
       </c>
       <c r="E7" t="n">
-        <v>31.12128529111659</v>
+        <v>867.1773319770334</v>
       </c>
       <c r="F7" t="n">
-        <v>11.58014932273346</v>
+        <v>456.848542737133</v>
       </c>
       <c r="G7" t="n">
-        <v>18.36717080568337</v>
+        <v>584.8295806411332</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>WaterUse</t>
+          <t>Acid</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>817.9715822192637</v>
+        <v>24.63724972834163</v>
       </c>
       <c r="C8" t="n">
-        <v>787.2341085736156</v>
+        <v>27.6967985072017</v>
       </c>
       <c r="D8" t="n">
-        <v>984.7551522402184</v>
+        <v>47.99286076401824</v>
       </c>
       <c r="E8" t="n">
-        <v>867.1773319770334</v>
+        <v>34.63325750122834</v>
       </c>
       <c r="F8" t="n">
-        <v>456.848542737133</v>
+        <v>11.67831689261419</v>
       </c>
       <c r="G8" t="n">
-        <v>584.8295806411332</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Acid</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>24.63724972834163</v>
-      </c>
-      <c r="C9" t="n">
-        <v>27.6967985072017</v>
-      </c>
-      <c r="D9" t="n">
-        <v>47.99286076401824</v>
-      </c>
-      <c r="E9" t="n">
-        <v>34.63325750122834</v>
-      </c>
-      <c r="F9" t="n">
-        <v>11.67831689261419</v>
-      </c>
-      <c r="G9" t="n">
         <v>22.08373726353167</v>
       </c>
     </row>

</xml_diff>